<commit_message>
commit files for project metrics
</commit_message>
<xml_diff>
--- a/plugins/project_metrics/download/dmo/DMO_Weekly_Report.xlsx
+++ b/plugins/project_metrics/download/dmo/DMO_Weekly_Report.xlsx
@@ -64,6 +64,7 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -89,7 +90,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
@@ -97,21 +98,6 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="thin">
-        <color rgb="FF3C3C3C"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3C3C3C"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3C3C3C"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3C3C3C"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="20">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
@@ -138,7 +124,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -151,20 +137,8 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="1" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="2" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -176,85 +150,13 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
   </cellStyles>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="FF000000"/>
-      <rgbColor rgb="FFFFFFFF"/>
-      <rgbColor rgb="FFFF0000"/>
-      <rgbColor rgb="FF00FF00"/>
-      <rgbColor rgb="FF0000FF"/>
-      <rgbColor rgb="FFFFFF00"/>
-      <rgbColor rgb="FFFF00FF"/>
-      <rgbColor rgb="FF00FFFF"/>
-      <rgbColor rgb="FF800000"/>
-      <rgbColor rgb="FF008000"/>
-      <rgbColor rgb="FF000080"/>
-      <rgbColor rgb="FF808000"/>
-      <rgbColor rgb="FF800080"/>
-      <rgbColor rgb="FF008080"/>
-      <rgbColor rgb="FFC0C0C0"/>
-      <rgbColor rgb="FF808080"/>
-      <rgbColor rgb="FF9999FF"/>
-      <rgbColor rgb="FF993366"/>
-      <rgbColor rgb="FFFFFFCC"/>
-      <rgbColor rgb="FFCCFFFF"/>
-      <rgbColor rgb="FF660066"/>
-      <rgbColor rgb="FFFF8080"/>
-      <rgbColor rgb="FF0066CC"/>
-      <rgbColor rgb="FFCCCCFF"/>
-      <rgbColor rgb="FF000080"/>
-      <rgbColor rgb="FFFF00FF"/>
-      <rgbColor rgb="FFFFFF00"/>
-      <rgbColor rgb="FF00FFFF"/>
-      <rgbColor rgb="FF800080"/>
-      <rgbColor rgb="FF800000"/>
-      <rgbColor rgb="FF008080"/>
-      <rgbColor rgb="FF0000FF"/>
-      <rgbColor rgb="FF00CCFF"/>
-      <rgbColor rgb="FFCCFFFF"/>
-      <rgbColor rgb="FFCCFFCC"/>
-      <rgbColor rgb="FFFFFF99"/>
-      <rgbColor rgb="FF99CCFF"/>
-      <rgbColor rgb="FFFF99CC"/>
-      <rgbColor rgb="FFCC99FF"/>
-      <rgbColor rgb="FFFFCC99"/>
-      <rgbColor rgb="FF3366FF"/>
-      <rgbColor rgb="FF33CCCC"/>
-      <rgbColor rgb="FF99CC00"/>
-      <rgbColor rgb="FFFFCC00"/>
-      <rgbColor rgb="FFFF9900"/>
-      <rgbColor rgb="FFFF6600"/>
-      <rgbColor rgb="FF666699"/>
-      <rgbColor rgb="FF969696"/>
-      <rgbColor rgb="FF003366"/>
-      <rgbColor rgb="FF339966"/>
-      <rgbColor rgb="FF003300"/>
-      <rgbColor rgb="FF333300"/>
-      <rgbColor rgb="FF993300"/>
-      <rgbColor rgb="FF993366"/>
-      <rgbColor rgb="FF333399"/>
-      <rgbColor rgb="FF3C3C3C"/>
-    </indexedColors>
-  </colors>
 </styleSheet>
-</file>
-
-<file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable3" cacheId="0" dataOnRows="false" dataPosition="65535" autoFormatId="1" dataCaption="Values" enableDrill="true" rowGrandTotals="true" colGrandTotals="true">
-  <location ref="I1:J7" firstHeaderRow="2" firstDataRow="3" firstDataCol="8" rowPageCount="4" colPageCount="2"/>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable2" cacheId="0" dataOnRows="false" dataPosition="65535" autoFormatId="1" dataCaption="Values" enableDrill="true" rowGrandTotals="true" colGrandTotals="true">
-  <location ref="A3:B12" firstHeaderRow="4" firstDataRow="5" firstDataCol="0" rowPageCount="7" colPageCount="2"/>
-</pivotTableDefinition>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
-    <tabColor rgb="00FFFFFF"/>
+    <tabColor rgb="FFFFFFFF"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:J12"/>
@@ -270,8 +172,10 @@
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="10.7125506072875"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="7.2834008097166"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="11.2834008097166"/>
+    <col collapsed="false" hidden="false" max="8" min="6" style="0" width="8.5748987854251"/>
     <col collapsed="false" hidden="false" max="9" min="9" style="0" width="13.1417004048583"/>
     <col collapsed="false" hidden="false" max="10" min="10" style="0" width="9.99595141700405"/>
+    <col collapsed="false" hidden="false" max="1025" min="11" style="0" width="8.5748987854251"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -300,27 +204,27 @@
       <c r="A4" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="3" t="n">
+      <c r="B4" s="0" t="n">
         <v>2</v>
       </c>
       <c r="I4" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="J4" s="3" t="n">
+      <c r="J4" s="0" t="n">
         <v>7</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="4" t="s">
+      <c r="A5" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="3" t="n">
+      <c r="B5" s="0" t="n">
         <v>2</v>
       </c>
       <c r="I5" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="J5" s="3" t="n">
+      <c r="J5" s="0" t="n">
         <v>2</v>
       </c>
     </row>
@@ -328,25 +232,24 @@
       <c r="A6" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="3" t="n">
+      <c r="B6" s="0" t="n">
         <v>2</v>
       </c>
       <c r="I6" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J6" s="3"/>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B7" s="3" t="n">
+      <c r="A7" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" s="0" t="n">
         <v>2</v>
       </c>
       <c r="I7" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="J7" s="3" t="n">
+      <c r="J7" s="0" t="n">
         <v>9</v>
       </c>
     </row>
@@ -354,15 +257,15 @@
       <c r="A8" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B8" s="3" t="n">
+      <c r="B8" s="0" t="n">
         <v>5</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B9" s="3" t="n">
+      <c r="A9" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B9" s="0" t="n">
         <v>5</v>
       </c>
     </row>
@@ -370,19 +273,17 @@
       <c r="A10" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B10" s="3"/>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="4" t="s">
+      <c r="A11" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="3"/>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B12" s="3" t="n">
+      <c r="B12" s="0" t="n">
         <v>9</v>
       </c>
     </row>
@@ -400,16 +301,16 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
-    <tabColor rgb="00FFFFFF"/>
+    <tabColor rgb="FFFFFFFF"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F10"/>
+  <dimension ref="A1"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D14" activeCellId="0" sqref="1:1048576"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="1:1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.8"/>
+  <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="7"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="11.7125506072874"/>
@@ -417,89 +318,9 @@
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="54.2753036437247"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="35.2793522267206"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="23.2793522267206"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.5748987854251"/>
   </cols>
-  <sheetData>
-    <row r="1" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="5"/>
-      <c r="B1" s="5"/>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5"/>
-    </row>
-    <row r="2" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="5"/>
-      <c r="B2" s="5"/>
-      <c r="C2" s="5"/>
-      <c r="D2" s="5"/>
-      <c r="E2" s="5"/>
-      <c r="F2" s="5"/>
-    </row>
-    <row r="3" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="5"/>
-      <c r="B3" s="5"/>
-      <c r="C3" s="5"/>
-      <c r="D3" s="5"/>
-      <c r="E3" s="5"/>
-      <c r="F3" s="5"/>
-    </row>
-    <row r="4" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="5"/>
-      <c r="B4" s="5"/>
-      <c r="C4" s="5"/>
-      <c r="D4" s="5"/>
-      <c r="E4" s="5"/>
-      <c r="F4" s="5"/>
-    </row>
-    <row r="5" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="5"/>
-      <c r="B5" s="5"/>
-      <c r="C5" s="5"/>
-      <c r="D5" s="5"/>
-      <c r="E5" s="5"/>
-      <c r="F5" s="5"/>
-    </row>
-    <row r="6" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="5"/>
-      <c r="B6" s="5"/>
-      <c r="C6" s="5"/>
-      <c r="D6" s="5"/>
-      <c r="E6" s="5"/>
-      <c r="F6" s="5"/>
-    </row>
-    <row r="7" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="5"/>
-      <c r="B7" s="5"/>
-      <c r="C7" s="5"/>
-      <c r="D7" s="5"/>
-      <c r="E7" s="5"/>
-      <c r="F7" s="5"/>
-    </row>
-    <row r="8" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="5"/>
-      <c r="B8" s="5"/>
-      <c r="C8" s="5"/>
-      <c r="D8" s="5"/>
-      <c r="E8" s="5"/>
-      <c r="F8" s="5"/>
-    </row>
-    <row r="9" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="5"/>
-      <c r="B9" s="5"/>
-      <c r="C9" s="5"/>
-      <c r="D9" s="5"/>
-      <c r="E9" s="5"/>
-      <c r="F9" s="6"/>
-    </row>
-    <row r="10" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="5"/>
-      <c r="B10" s="5"/>
-      <c r="C10" s="5"/>
-      <c r="D10" s="5"/>
-      <c r="E10" s="5"/>
-      <c r="F10" s="5"/>
-    </row>
-  </sheetData>
+  <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>